<commit_message>
fixing mother cell notation
</commit_message>
<xml_diff>
--- a/data/derived/Fig5 dividing cells.xlsx
+++ b/data/derived/Fig5 dividing cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maddie/GitHub/KSHV_mathematical_analysis/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55761C73-7946-AC44-BEC9-1EBB23AF7410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E21F0CFC-06C5-F144-8AC8-5DAC36C500E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2180" windowWidth="25920" windowHeight="17120" xr2:uid="{D9AFDDD2-5302-4967-8D1F-764C5A819ED0}"/>
+    <workbookView xWindow="11980" yWindow="3460" windowWidth="25920" windowHeight="17120" xr2:uid="{D9AFDDD2-5302-4967-8D1F-764C5A819ED0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Image 1</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Image 14</t>
   </si>
   <si>
-    <t>Image 15</t>
-  </si>
-  <si>
     <t>Image 16</t>
   </si>
   <si>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>Total cluster intensity_daughter2</t>
+  </si>
+  <si>
+    <t>Image 15.1</t>
+  </si>
+  <si>
+    <t>Image 15.2</t>
   </si>
 </sst>
 </file>
@@ -678,32 +681,32 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1020,7 +1023,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
@@ -1043,7 +1046,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B17" s="11">
         <v>1</v>
@@ -1066,7 +1069,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -1089,7 +1092,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -1135,7 +1138,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -1181,7 +1184,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -1204,7 +1207,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -1227,7 +1230,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -1250,7 +1253,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -1273,7 +1276,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
@@ -1296,7 +1299,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -1319,7 +1322,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -1338,7 +1341,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -1357,7 +1360,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="8">
         <v>1</v>
@@ -1380,7 +1383,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1395,7 +1398,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="11">
         <v>3</v>
@@ -1412,7 +1415,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -1435,7 +1438,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -1481,7 +1484,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>

</xml_diff>